<commit_message>
- small fix in metadata change tracking
</commit_message>
<xml_diff>
--- a/template_v4_test.xlsx
+++ b/template_v4_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>Metadata</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Name:</t>
   </si>
   <si>
-    <t>Some Researcher</t>
+    <t>Some Optimistic Researcher</t>
   </si>
   <si>
     <t>Optional Upload Comments:</t>
@@ -303,6 +303,15 @@
   </si>
   <si>
     <t>P4</t>
+  </si>
+  <si>
+    <t>BNAl</t>
+  </si>
+  <si>
+    <t>HCP</t>
+  </si>
+  <si>
+    <t>Researcher_2024_SomeNicePaper</t>
   </si>
 </sst>
 </file>
@@ -1820,8 +1829,12 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="74"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
       <c r="F11" s="4"/>
@@ -1832,7 +1845,9 @@
       <c r="K11" s="77"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="N11" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="O11" s="5"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>

</xml_diff>